<commit_message>
Added latest DB snapshot
</commit_message>
<xml_diff>
--- a/Design/LLD_PatientTracker.xlsx
+++ b/Design/LLD_PatientTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riyad\Documents\MSCS\Fall_2023\520\Project\PatientTrackerSystem\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1255362-2097-4045-B67A-56975639529E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579276B1-2D74-46F4-9FA3-34AB92D681CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{B16DD8E1-169D-490C-9B29-CB84FEC806A4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B16DD8E1-169D-490C-9B29-CB84FEC806A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="190">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -821,6 +821,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -878,8 +880,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1845,11 +1845,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C6" s="4" t="s">
@@ -1919,11 +1919,11 @@
       <c r="E12" s="4"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C16" s="4" t="s">
@@ -2002,11 +2002,11 @@
       <c r="E23" s="1"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C27" s="4" t="s">
@@ -2096,11 +2096,11 @@
       <c r="E35" s="1"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="24"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C39" s="4" t="s">
@@ -2253,11 +2253,11 @@
       <c r="E54" s="1"/>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="26"/>
-      <c r="E56" s="27"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="29"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C57" s="4" t="s">
@@ -2309,11 +2309,11 @@
       <c r="E61" s="1"/>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C63" s="21" t="s">
+      <c r="C63" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C64" s="4" t="s">
@@ -2400,11 +2400,11 @@
       <c r="E71" s="1"/>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C74" s="5" t="s">
@@ -2541,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6A6E98-AD5D-4B53-BABA-5087D4A6A66C}">
   <dimension ref="C1:P43"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="84" x14ac:dyDescent="1.8"/>
@@ -2568,21 +2568,21 @@
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="3:16" x14ac:dyDescent="1.8">
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
-      <c r="I2" s="33" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="I2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="35"/>
-      <c r="N2" s="33" t="s">
+      <c r="J2" s="36"/>
+      <c r="K2" s="37"/>
+      <c r="N2" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="1.8">
       <c r="C3" s="10" t="s">
@@ -2728,11 +2728,11 @@
       <c r="P8" s="15"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="1.8">
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="I9" s="7" t="s">
         <v>26</v>
       </c>
@@ -2821,16 +2821,16 @@
         <v>103</v>
       </c>
       <c r="E13" s="16"/>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="N13" s="32" t="s">
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="N13" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
     </row>
     <row r="14" spans="3:16" ht="168" x14ac:dyDescent="1.8">
       <c r="C14" s="7" t="s">
@@ -2932,11 +2932,11 @@
       </c>
     </row>
     <row r="18" spans="3:16" ht="168" x14ac:dyDescent="1.8">
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
       <c r="I18" s="7" t="s">
         <v>41</v>
       </c>
@@ -3113,7 +3113,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3161,8 +3161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7A1C85-8F70-44AB-806A-D73715F37D2D}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3199,7 +3199,7 @@
       <c r="A2" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="20" t="s">
         <v>133</v>
       </c>
       <c r="C2" t="s">
@@ -3211,7 +3211,7 @@
       <c r="E2">
         <v>4364526060</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="20" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3219,7 +3219,7 @@
       <c r="A3" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="20" t="s">
         <v>134</v>
       </c>
       <c r="C3" t="s">
@@ -3231,7 +3231,7 @@
       <c r="E3">
         <v>6473589678</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="20" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3239,7 +3239,7 @@
       <c r="A4" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="20" t="s">
         <v>135</v>
       </c>
       <c r="C4" t="s">
@@ -3251,7 +3251,7 @@
       <c r="E4">
         <v>4138898787</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="20" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
       <c r="A5" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="20" t="s">
         <v>136</v>
       </c>
       <c r="C5" t="s">
@@ -3271,7 +3271,7 @@
       <c r="E5">
         <v>7268672345</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="20" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3279,7 +3279,7 @@
       <c r="A6" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="20" t="s">
         <v>137</v>
       </c>
       <c r="C6" t="s">
@@ -3291,7 +3291,7 @@
       <c r="E6">
         <v>5678932211</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="20" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3299,7 +3299,7 @@
       <c r="A7" t="s">
         <v>147</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="20" t="s">
         <v>138</v>
       </c>
       <c r="C7" t="s">
@@ -3311,7 +3311,7 @@
       <c r="E7">
         <v>8769761212</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="20" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3319,7 +3319,7 @@
       <c r="A8" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="20" t="s">
         <v>139</v>
       </c>
       <c r="C8" t="s">
@@ -3331,7 +3331,7 @@
       <c r="E8">
         <v>3214567890</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="20" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3339,7 +3339,7 @@
       <c r="A9" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="20" t="s">
         <v>140</v>
       </c>
       <c r="C9" t="s">
@@ -3351,7 +3351,7 @@
       <c r="E9">
         <v>1234567890</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="20" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3359,7 +3359,7 @@
       <c r="A10" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="20" t="s">
         <v>141</v>
       </c>
       <c r="C10" t="s">
@@ -3371,7 +3371,7 @@
       <c r="E10">
         <v>2123546798</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="20" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3379,7 +3379,7 @@
       <c r="A11" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="20" t="s">
         <v>142</v>
       </c>
       <c r="C11" t="s">
@@ -3391,7 +3391,7 @@
       <c r="E11">
         <v>4568906565</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="20" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       <c r="A12" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="20" t="s">
         <v>132</v>
       </c>
       <c r="C12" t="s">
@@ -3411,7 +3411,7 @@
       <c r="E12">
         <v>1239087635</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="20" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3450,7 +3450,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3491,7 +3491,7 @@
       <c r="A2" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="20" t="s">
         <v>174</v>
       </c>
       <c r="C2" t="s">
@@ -3503,7 +3503,7 @@
       <c r="E2">
         <v>1233214567</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="20" t="s">
         <v>174</v>
       </c>
       <c r="G2" t="s">
@@ -3514,7 +3514,7 @@
       <c r="A3" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C3" t="s">
@@ -3526,7 +3526,7 @@
       <c r="E3">
         <v>9876541234</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="20" t="s">
         <v>175</v>
       </c>
       <c r="G3" t="s">
@@ -3537,7 +3537,7 @@
       <c r="A4" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="20" t="s">
         <v>176</v>
       </c>
       <c r="C4" t="s">
@@ -3549,7 +3549,7 @@
       <c r="E4">
         <v>6785431298</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="20" t="s">
         <v>176</v>
       </c>
       <c r="G4" t="s">
@@ -3560,7 +3560,7 @@
       <c r="A5" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="20" t="s">
         <v>177</v>
       </c>
       <c r="C5" t="s">
@@ -3572,7 +3572,7 @@
       <c r="E5">
         <v>6743126767</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="20" t="s">
         <v>177</v>
       </c>
       <c r="G5" t="s">
@@ -3583,7 +3583,7 @@
       <c r="A6" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="20" t="s">
         <v>178</v>
       </c>
       <c r="C6" t="s">
@@ -3595,7 +3595,7 @@
       <c r="E6">
         <v>8822994411</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="20" t="s">
         <v>178</v>
       </c>
       <c r="G6" t="s">
@@ -3624,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4DF7A3-D6CB-4D45-94C3-50D1E4AEDAFA}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3678,7 +3678,7 @@
       <c r="E2">
         <v>28</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="21">
         <v>45205</v>
       </c>
       <c r="G2" t="s">
@@ -3701,7 +3701,7 @@
       <c r="E3">
         <v>28</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="21">
         <v>45245</v>
       </c>
       <c r="G3" t="s">
@@ -3724,7 +3724,7 @@
       <c r="E4">
         <v>28</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="21">
         <v>45269</v>
       </c>
       <c r="G4" t="s">
@@ -3747,7 +3747,7 @@
       <c r="E5">
         <v>25</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="21">
         <v>45178</v>
       </c>
       <c r="G5" t="s">
@@ -3770,7 +3770,7 @@
       <c r="E6">
         <v>25</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="21">
         <v>45208</v>
       </c>
       <c r="G6" t="s">
@@ -3793,7 +3793,7 @@
       <c r="E7">
         <v>25</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="21">
         <v>45239</v>
       </c>
       <c r="G7" t="s">
@@ -3816,7 +3816,7 @@
       <c r="E8">
         <v>45</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="21">
         <v>44927</v>
       </c>
       <c r="G8" t="s">
@@ -3839,7 +3839,7 @@
       <c r="E9">
         <v>46</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="21">
         <v>45049</v>
       </c>
       <c r="G9" t="s">
@@ -3862,7 +3862,7 @@
       <c r="E10">
         <v>46</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="21">
         <v>45270</v>
       </c>
       <c r="G10" t="s">
@@ -3885,8 +3885,11 @@
       <c r="E11">
         <v>12</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="21">
         <v>45031</v>
+      </c>
+      <c r="G11" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -3905,8 +3908,11 @@
       <c r="E12">
         <v>12</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="21">
         <v>45185</v>
+      </c>
+      <c r="G12" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -3925,8 +3931,11 @@
       <c r="E13">
         <v>12</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="21">
         <v>45267</v>
+      </c>
+      <c r="G13" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -3945,8 +3954,11 @@
       <c r="E14">
         <v>32</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="21">
         <v>45000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -3965,8 +3977,11 @@
       <c r="E15">
         <v>32</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="21">
         <v>45038</v>
+      </c>
+      <c r="G15" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -3985,8 +4000,11 @@
       <c r="E16">
         <v>33</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="21">
         <v>45048</v>
+      </c>
+      <c r="G16" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated records and inserted data for two tables
</commit_message>
<xml_diff>
--- a/Design/LLD_PatientTracker.xlsx
+++ b/Design/LLD_PatientTracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riyad\Documents\MSCS\Fall_2023\520\Project\PatientTrackerSystem\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riya\UMass\Fall23\520\PatientTrackerSystem\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579276B1-2D74-46F4-9FA3-34AB92D681CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD61C6F-92EA-40DC-BDC4-8BDA08FFC2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B16DD8E1-169D-490C-9B29-CB84FEC806A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="7" xr2:uid="{B16DD8E1-169D-490C-9B29-CB84FEC806A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Patient_Master" sheetId="4" r:id="rId4"/>
     <sheet name="Doctor_Master" sheetId="5" r:id="rId5"/>
     <sheet name="Patient_General_Demographics" sheetId="6" r:id="rId6"/>
+    <sheet name="Health_History_Master" sheetId="7" r:id="rId7"/>
+    <sheet name="Appointment_Master" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="194">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -619,6 +621,18 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Time_of_Appointment</t>
+  </si>
+  <si>
+    <t>Confirnmed</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Date_of_Measurement</t>
   </si>
 </sst>
 </file>
@@ -768,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -880,6 +894,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1837,21 +1852,21 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.08984375" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="24" t="s">
         <v>62</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="26"/>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1862,7 +1877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
@@ -1873,7 +1888,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>100</v>
       </c>
@@ -1882,7 +1897,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>101</v>
       </c>
@@ -1891,7 +1906,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
@@ -1900,7 +1915,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
@@ -1909,7 +1924,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>3</v>
       </c>
@@ -1918,14 +1933,14 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" s="24" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +1951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
         <v>12</v>
       </c>
@@ -1947,7 +1962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="5" t="s">
         <v>104</v>
       </c>
@@ -1956,7 +1971,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
         <v>106</v>
       </c>
@@ -1965,7 +1980,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
         <v>13</v>
       </c>
@@ -1974,7 +1989,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
@@ -1983,7 +1998,7 @@
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="5" t="s">
         <v>15</v>
       </c>
@@ -1992,7 +2007,7 @@
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="3:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:5" ht="75" x14ac:dyDescent="0.25">
       <c r="C23" s="5" t="s">
         <v>16</v>
       </c>
@@ -2001,14 +2016,14 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="26"/>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>4</v>
       </c>
@@ -2019,7 +2034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
         <v>0</v>
       </c>
@@ -2030,7 +2045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>22</v>
       </c>
@@ -2039,7 +2054,7 @@
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
         <v>23</v>
       </c>
@@ -2048,7 +2063,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C31" s="5" t="s">
         <v>24</v>
       </c>
@@ -2057,7 +2072,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C32" s="5" t="s">
         <v>25</v>
       </c>
@@ -2066,7 +2081,7 @@
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="5" t="s">
         <v>26</v>
       </c>
@@ -2075,7 +2090,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
         <v>37</v>
       </c>
@@ -2086,7 +2101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>38</v>
       </c>
@@ -2095,14 +2110,14 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" s="24" t="s">
         <v>35</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="26"/>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C40" s="5" t="s">
         <v>0</v>
       </c>
@@ -2124,7 +2139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C41" s="5" t="s">
         <v>12</v>
       </c>
@@ -2135,7 +2150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
         <v>39</v>
       </c>
@@ -2144,7 +2159,7 @@
       </c>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
         <v>41</v>
       </c>
@@ -2153,7 +2168,7 @@
       </c>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
         <v>44</v>
       </c>
@@ -2162,7 +2177,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
         <v>46</v>
       </c>
@@ -2171,7 +2186,7 @@
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C46" s="5" t="s">
         <v>47</v>
       </c>
@@ -2180,7 +2195,7 @@
       </c>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C47" s="5" t="s">
         <v>48</v>
       </c>
@@ -2189,7 +2204,7 @@
       </c>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C48" s="5" t="s">
         <v>49</v>
       </c>
@@ -2198,7 +2213,7 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C49" s="5" t="s">
         <v>50</v>
       </c>
@@ -2207,7 +2222,7 @@
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" s="5" t="s">
         <v>51</v>
       </c>
@@ -2216,7 +2231,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" s="5" t="s">
         <v>53</v>
       </c>
@@ -2225,7 +2240,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="5" t="s">
         <v>55</v>
       </c>
@@ -2234,7 +2249,7 @@
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" s="5" t="s">
         <v>56</v>
       </c>
@@ -2243,7 +2258,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" s="5" t="s">
         <v>57</v>
       </c>
@@ -2252,14 +2267,14 @@
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" s="27" t="s">
         <v>61</v>
       </c>
       <c r="D56" s="28"/>
       <c r="E56" s="29"/>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57" s="4" t="s">
         <v>4</v>
       </c>
@@ -2270,7 +2285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>64</v>
       </c>
@@ -2281,7 +2296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
         <v>65</v>
       </c>
@@ -2290,7 +2305,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="1" t="s">
         <v>108</v>
       </c>
@@ -2299,7 +2314,7 @@
       </c>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
         <v>109</v>
       </c>
@@ -2308,14 +2323,14 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" s="23" t="s">
         <v>68</v>
       </c>
       <c r="D63" s="23"/>
       <c r="E63" s="23"/>
     </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" s="4" t="s">
         <v>4</v>
       </c>
@@ -2326,7 +2341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C65" s="5" t="s">
         <v>69</v>
       </c>
@@ -2337,7 +2352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66" s="5" t="s">
         <v>0</v>
       </c>
@@ -2348,7 +2363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C67" s="5" t="s">
         <v>12</v>
       </c>
@@ -2359,7 +2374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C68" s="5" t="s">
         <v>70</v>
       </c>
@@ -2370,7 +2385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C69" s="5" t="s">
         <v>71</v>
       </c>
@@ -2381,7 +2396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C70" s="5" t="s">
         <v>79</v>
       </c>
@@ -2390,7 +2405,7 @@
       </c>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="3:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:5" ht="105" x14ac:dyDescent="0.25">
       <c r="C71" s="5" t="s">
         <v>72</v>
       </c>
@@ -2399,14 +2414,14 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73" s="22" t="s">
         <v>81</v>
       </c>
       <c r="D73" s="22"/>
       <c r="E73" s="22"/>
     </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C74" s="5" t="s">
         <v>4</v>
       </c>
@@ -2417,7 +2432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C75" s="5" t="s">
         <v>0</v>
       </c>
@@ -2428,7 +2443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C76" s="5" t="s">
         <v>88</v>
       </c>
@@ -2437,7 +2452,7 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C77" s="5" t="s">
         <v>89</v>
       </c>
@@ -2446,7 +2461,7 @@
       </c>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C78" s="5" t="s">
         <v>82</v>
       </c>
@@ -2455,7 +2470,7 @@
       </c>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C79" s="5" t="s">
         <v>83</v>
       </c>
@@ -2464,7 +2479,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C80" s="5" t="s">
         <v>84</v>
       </c>
@@ -2473,7 +2488,7 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81" s="5" t="s">
         <v>85</v>
       </c>
@@ -2482,7 +2497,7 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C82" s="5" t="s">
         <v>86</v>
       </c>
@@ -2491,7 +2506,7 @@
       </c>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C83" s="5" t="s">
         <v>87</v>
       </c>
@@ -2500,7 +2515,7 @@
       </c>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="3:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C84" s="5" t="s">
         <v>36</v>
       </c>
@@ -2511,7 +2526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C85" s="5" t="s">
         <v>98</v>
       </c>
@@ -2541,33 +2556,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6A6E98-AD5D-4B53-BABA-5087D4A6A66C}">
   <dimension ref="C1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="84" x14ac:dyDescent="1.8"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="84.75" x14ac:dyDescent="1.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="8"/>
-    <col min="3" max="3" width="128.7265625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="250.54296875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="75.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="8"/>
-    <col min="8" max="8" width="105.08984375" style="8" customWidth="1"/>
-    <col min="9" max="9" width="135.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="255.08984375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="75.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="8"/>
+    <col min="1" max="2" width="8.7109375" style="8"/>
+    <col min="3" max="3" width="128.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="250.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="75.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" style="8"/>
+    <col min="8" max="8" width="105.140625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="135.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="255.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="75.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="8"/>
     <col min="13" max="13" width="126" style="8" customWidth="1"/>
-    <col min="14" max="14" width="122.36328125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="255.54296875" style="8" customWidth="1"/>
-    <col min="16" max="16" width="75.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.7265625" style="8"/>
+    <col min="14" max="14" width="122.42578125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="255.5703125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="75.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="1" spans="3:16" x14ac:dyDescent="1.25">
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="2" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C2" s="38" t="s">
         <v>61</v>
       </c>
@@ -2584,7 +2599,7 @@
       <c r="O2" s="36"/>
       <c r="P2" s="37"/>
     </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="3" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
@@ -2613,7 +2628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="4" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C4" s="14" t="s">
         <v>64</v>
       </c>
@@ -2642,7 +2657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="5" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C5" s="14" t="s">
         <v>65</v>
       </c>
@@ -2665,7 +2680,7 @@
       </c>
       <c r="P5" s="15"/>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="6" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C6" s="14" t="s">
         <v>108</v>
       </c>
@@ -2688,7 +2703,7 @@
       </c>
       <c r="P6" s="15"/>
     </row>
-    <row r="7" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="7" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C7" s="14" t="s">
         <v>109</v>
       </c>
@@ -2711,7 +2726,7 @@
       </c>
       <c r="P7" s="15"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="8" spans="3:16" x14ac:dyDescent="1.25">
       <c r="I8" s="7" t="s">
         <v>25</v>
       </c>
@@ -2727,7 +2742,7 @@
       </c>
       <c r="P8" s="15"/>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="9" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C9" s="30" t="s">
         <v>62</v>
       </c>
@@ -2750,7 +2765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="10" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C10" s="10" t="s">
         <v>4</v>
       </c>
@@ -2779,7 +2794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="11" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C11" s="7" t="s">
         <v>0</v>
       </c>
@@ -2804,7 +2819,7 @@
       </c>
       <c r="P11" s="14"/>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="12" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C12" s="7" t="s">
         <v>100</v>
       </c>
@@ -2813,7 +2828,7 @@
       </c>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="13" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C13" s="7" t="s">
         <v>101</v>
       </c>
@@ -2832,7 +2847,7 @@
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
     </row>
-    <row r="14" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="14" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C14" s="7" t="s">
         <v>1</v>
       </c>
@@ -2859,7 +2874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="15" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C15" s="7" t="s">
         <v>2</v>
       </c>
@@ -2886,7 +2901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="16" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C16" s="7" t="s">
         <v>3</v>
       </c>
@@ -2913,7 +2928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="17" spans="3:16" x14ac:dyDescent="1.25">
       <c r="I17" s="7" t="s">
         <v>39</v>
       </c>
@@ -2931,7 +2946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="18" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C18" s="30" t="s">
         <v>63</v>
       </c>
@@ -2954,7 +2969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="19" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C19" s="10" t="s">
         <v>4</v>
       </c>
@@ -2981,7 +2996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="20" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C20" s="7" t="s">
         <v>12</v>
       </c>
@@ -3006,7 +3021,7 @@
       </c>
       <c r="P20" s="15"/>
     </row>
-    <row r="21" spans="3:16" ht="252" x14ac:dyDescent="1.8">
+    <row r="21" spans="3:16" ht="254.25" x14ac:dyDescent="1.25">
       <c r="C21" s="7" t="s">
         <v>104</v>
       </c>
@@ -3029,7 +3044,7 @@
       </c>
       <c r="P21" s="14"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="22" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C22" s="7" t="s">
         <v>106</v>
       </c>
@@ -3045,7 +3060,7 @@
       </c>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="23" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C23" s="7" t="s">
         <v>13</v>
       </c>
@@ -3061,7 +3076,7 @@
       </c>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="24" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C24" s="7" t="s">
         <v>14</v>
       </c>
@@ -3071,7 +3086,7 @@
       <c r="E24" s="16"/>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="1.8">
+    <row r="25" spans="3:16" x14ac:dyDescent="1.25">
       <c r="C25" s="7" t="s">
         <v>15</v>
       </c>
@@ -3080,7 +3095,7 @@
       </c>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="3:16" ht="168" x14ac:dyDescent="1.8">
+    <row r="26" spans="3:16" ht="169.5" x14ac:dyDescent="1.25">
       <c r="C26" s="7" t="s">
         <v>16</v>
       </c>
@@ -3089,7 +3104,7 @@
       </c>
       <c r="E26" s="14"/>
     </row>
-    <row r="43" spans="9:10" x14ac:dyDescent="1.8">
+    <row r="43" spans="9:10" x14ac:dyDescent="1.25">
       <c r="I43" s="9"/>
       <c r="J43" s="19"/>
     </row>
@@ -3116,15 +3131,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3138,7 +3153,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -3165,17 +3180,17 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
-    <col min="5" max="5" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3215,7 +3230,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -3235,7 +3250,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>144</v>
       </c>
@@ -3255,7 +3270,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -3275,7 +3290,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -3295,7 +3310,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -3315,7 +3330,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -3335,7 +3350,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -3355,7 +3370,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -3375,7 +3390,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>151</v>
       </c>
@@ -3395,7 +3410,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -3453,18 +3468,18 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.7265625" customWidth="1"/>
-    <col min="7" max="7" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3487,7 +3502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>164</v>
       </c>
@@ -3510,7 +3525,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -3533,7 +3548,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -3556,7 +3571,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -3579,7 +3594,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3624,22 +3639,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4DF7A3-D6CB-4D45-94C3-50D1E4AEDAFA}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3662,7 +3677,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -3685,7 +3700,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -3708,7 +3723,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -3731,7 +3746,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -3754,7 +3769,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>143</v>
       </c>
@@ -3777,7 +3792,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -3800,7 +3815,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -3823,7 +3838,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>144</v>
       </c>
@@ -3846,7 +3861,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -3869,7 +3884,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -3892,7 +3907,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -3915,7 +3930,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -3938,7 +3953,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -3961,7 +3976,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -3984,7 +3999,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -4007,92 +4022,92 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>152</v>
       </c>
@@ -4101,4 +4116,320 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D8CA44-6451-4B23-89BA-54B76BD17833}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2">
+        <v>110</v>
+      </c>
+      <c r="C2">
+        <v>77</v>
+      </c>
+      <c r="D2">
+        <v>126</v>
+      </c>
+      <c r="E2">
+        <v>13.3</v>
+      </c>
+      <c r="F2" s="21">
+        <v>45268</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>116</v>
+      </c>
+      <c r="C3">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>130</v>
+      </c>
+      <c r="E3">
+        <v>12.2</v>
+      </c>
+      <c r="F3" s="21">
+        <v>45268</v>
+      </c>
+      <c r="G3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4">
+        <v>119</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>132</v>
+      </c>
+      <c r="E4">
+        <v>14.8</v>
+      </c>
+      <c r="F4" s="21">
+        <v>45268</v>
+      </c>
+      <c r="G4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5">
+        <v>124</v>
+      </c>
+      <c r="C5">
+        <v>73</v>
+      </c>
+      <c r="D5">
+        <v>120</v>
+      </c>
+      <c r="E5">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F5" s="21">
+        <v>45270</v>
+      </c>
+      <c r="G5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6">
+        <v>106</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>116</v>
+      </c>
+      <c r="E6">
+        <v>11.4</v>
+      </c>
+      <c r="F6" s="21">
+        <v>45270</v>
+      </c>
+      <c r="G6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEEBFFC-CD12-4A2D-B021-872D40D2798C}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="21">
+        <v>45268</v>
+      </c>
+      <c r="D2" s="41">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E2" s="41">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="21">
+        <v>45268</v>
+      </c>
+      <c r="D3" s="41">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E3" s="41">
+        <v>0.15625</v>
+      </c>
+      <c r="F3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="21">
+        <v>45269</v>
+      </c>
+      <c r="D4" s="41">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E4" s="41">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="F4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="21">
+        <v>45269</v>
+      </c>
+      <c r="D5" s="41">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E5" s="41">
+        <v>0.6875</v>
+      </c>
+      <c r="F5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="21">
+        <v>45272</v>
+      </c>
+      <c r="D6" s="41">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E6" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>